<commit_message>
add customer ui and guest ui
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\IdeaProject\Coffee_shop\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\IdeaProjects\Coffee_shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6F6C55-80A5-48FA-A2F1-CA7D1A54D2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32522D05-0EA0-416D-B547-0A579CCBFB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="1875" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUser" sheetId="1" r:id="rId1"/>
@@ -524,12 +524,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="11.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -557,7 +557,7 @@
         <v>13100008888</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,7 +567,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -587,7 +587,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -597,7 +597,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -621,17 +621,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -671,13 +671,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>123</v>
+        <v>123456</v>
       </c>
       <c r="G2" s="1">
         <v>15120065365</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -693,10 +693,12 @@
       <c r="E3" s="1">
         <v>10</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>123456</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -719,7 +721,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -756,13 +758,13 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,7 +781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -796,7 +798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -813,7 +815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -844,14 +846,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -885,7 +887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -912,18 +914,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,7 +945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -963,7 +965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
add dao insert and select
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\IdeaProjects\Coffee_shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32522D05-0EA0-416D-B547-0A579CCBFB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77CAEB8-6D86-4872-A82A-79314DCED538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="1875" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="1875" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUser" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -86,55 +86,16 @@
     <t>Mocca</t>
   </si>
   <si>
-    <t>RMB 30</t>
-  </si>
-  <si>
-    <t>100(库存)</t>
-  </si>
-  <si>
-    <t>20(销量)</t>
-  </si>
-  <si>
     <t>Cappuccino</t>
   </si>
   <si>
-    <t>RMB 32</t>
-  </si>
-  <si>
-    <t>200(库存)</t>
-  </si>
-  <si>
-    <t>40(销量)</t>
-  </si>
-  <si>
     <t>Latte</t>
   </si>
   <si>
-    <t>RMB 36</t>
-  </si>
-  <si>
-    <t>180(库存)</t>
-  </si>
-  <si>
-    <t>50(销量)</t>
-  </si>
-  <si>
     <t>ice cream</t>
   </si>
   <si>
-    <t>RMB 10</t>
-  </si>
-  <si>
-    <t>30(销量)</t>
-  </si>
-  <si>
     <t>cake</t>
-  </si>
-  <si>
-    <t>RMB 20</t>
-  </si>
-  <si>
-    <t>150(库存)</t>
   </si>
   <si>
     <t>bookDate</t>
@@ -175,6 +136,21 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>wyw</t>
+  </si>
+  <si>
+    <t>binghongcha</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>cookie</t>
   </si>
 </sst>
 </file>
@@ -526,7 +502,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="11.875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="11.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -537,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -599,16 +575,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -619,16 +595,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -703,22 +679,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -726,22 +702,45 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -752,16 +751,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -788,14 +787,14 @@
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -803,16 +802,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>200</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -820,16 +819,33 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1">
+        <v>180</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -840,17 +856,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="10.625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="10.625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -875,16 +891,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>200</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -892,16 +908,33 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>150</v>
+      </c>
+      <c r="E3" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -920,9 +953,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="24.375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="24.375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -936,13 +969,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -950,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1">
         <v>188</v>
@@ -970,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>288</v>

</xml_diff>

<commit_message>
add phone number in register some text in user interface are modified
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="131">
   <si>
     <t>id</t>
   </si>
@@ -262,6 +262,156 @@
   </si>
   <si>
     <t>96</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>yolanda</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>12332112345</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>234567</t>
+  </si>
+  <si>
+    <t>12345678901</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1468,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
@@ -1443,6 +1593,52 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1452,7 +1648,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1543,9 +1739,26 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1593,33 +1806,33 @@
         <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3">
-        <v>150</v>
-      </c>
-      <c r="E3" s="3">
-        <v>50</v>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
solved problem about become VIP
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>2022-12-11</t>
+  </si>
+  <si>
+    <t>188.0</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1654,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1743,23 +1749,6 @@
       </c>
       <c r="E5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1895,23 +1884,23 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3">
-        <v>188</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44919</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>10</v>
+      <c r="C2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
update new file(Database) to solve the conflict
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -264,16 +264,160 @@
     <t>96</t>
   </si>
   <si>
-    <t>666.0</t>
-  </si>
-  <si>
-    <t>78.0</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>Orange</t>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>yolanda</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>12332112345</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>234567</t>
+  </si>
+  <si>
+    <t>12345678901</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>2022-12-11</t>
+  </si>
+  <si>
+    <t>188.0</t>
   </si>
 </sst>
 </file>
@@ -1330,7 +1474,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
@@ -1455,6 +1599,52 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1464,7 +1654,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1555,27 +1745,10 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1628,27 +1801,27 @@
         <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3">
-        <v>150</v>
-      </c>
-      <c r="E3" s="3">
-        <v>50</v>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4">
@@ -1711,23 +1884,23 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3">
-        <v>188</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44919</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>10</v>
+      <c r="C2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
solved problem about gender setting
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -418,6 +418,15 @@
   </si>
   <si>
     <t>188.0</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>12234567890</t>
   </si>
 </sst>
 </file>
@@ -1601,48 +1610,48 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>85</v>
       </c>
       <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug about SalesRecord
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="145">
   <si>
     <t>id</t>
   </si>
@@ -436,6 +436,24 @@
   </si>
   <si>
     <t>998</t>
+  </si>
+  <si>
+    <t>Daven</t>
+  </si>
+  <si>
+    <t>SECRET</t>
+  </si>
+  <si>
+    <t>13117826002</t>
+  </si>
+  <si>
+    <t>997</t>
+  </si>
+  <si>
+    <t>996</t>
+  </si>
+  <si>
+    <t>-2</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1510,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
@@ -1661,6 +1679,29 @@
       </c>
       <c r="G7" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1763,10 +1804,10 @@
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1951,7 +1992,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G2"/>
@@ -2103,6 +2144,29 @@
         <v>131</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
delete one queryDrink() in buyDrink
</commit_message>
<xml_diff>
--- a/src/main/resources/Database.xlsx
+++ b/src/main/resources/Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -418,6 +418,36 @@
   </si>
   <si>
     <t>188.0</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>997</t>
+  </si>
+  <si>
+    <t>32.0</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>995</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>95</t>
   </si>
 </sst>
 </file>
@@ -1694,27 +1724,27 @@
         <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="3">
-        <v>32</v>
-      </c>
-      <c r="D3" s="3">
-        <v>200</v>
-      </c>
-      <c r="E3" s="3">
-        <v>40</v>
+      <c r="C3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1801,10 +1831,10 @@
         <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1818,10 +1848,10 @@
         <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">

</xml_diff>